<commit_message>
Update hotel prices and scores
</commit_message>
<xml_diff>
--- a/data/out/all_hotels.xlsx
+++ b/data/out/all_hotels.xlsx
@@ -463,71 +463,71 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>City Inn Paris</t>
+          <t>Austin's Saint Lazare Hotel</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>US$608</t>
+          <t>US$3,534</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>6.7</t>
+          <t>8.1</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Review score</t>
+          <t>Very Good</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2,498</t>
+          <t>2,540</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Hôtel des Andelys</t>
+          <t>Austin's Arts Et Metiers Hotel</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>US$1,423</t>
+          <t>US$3,971</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>4.0</t>
+          <t>8.2</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Review score</t>
+          <t>Very Good</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>929</t>
+          <t>2,030</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Austin's Saint Lazare Hotel</t>
+          <t>Apart hotel Le Marais Centre de Paris</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>US$3,534</t>
+          <t>US$4,613</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>8.1</t>
+          <t>8.0</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -537,78 +537,78 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>2,540</t>
+          <t>163</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Printania Porte de Versailles</t>
+          <t>Hotel Puy De Dôme</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>US$1,948</t>
+          <t>US$3,771</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>5.7</t>
+          <t>8.1</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Review score</t>
+          <t>Very Good</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>1,284</t>
+          <t>1,637</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Auriane Porte De Versailles</t>
+          <t>Hotel Anya</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>US$1,948</t>
+          <t>US$1,918</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>5.6</t>
+          <t>7.4</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Review score</t>
+          <t>Good</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>1,636</t>
+          <t>1,132</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Zoku Paris</t>
+          <t>PARIS AUTHENTIC HOUSE, Entier 1920's villa métro Line 7</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>US$3,315</t>
+          <t>US$10,710</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>9.1</t>
+          <t>9.4</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -618,78 +618,78 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>887</t>
+          <t>10</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>hotel azur</t>
+          <t>Zoku Paris</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>US$1,823</t>
+          <t>US$3,315</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>9.1</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Review score</t>
+          <t>Wonderful</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>887</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Hotel de France 18</t>
+          <t>Glasgow Monceau by Patrick Hayat</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>US$1,279</t>
+          <t>US$2,897</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>6.0</t>
+          <t>8.0</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Review score</t>
+          <t>Very Good</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>1,891</t>
+          <t>674</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Austin's Arts Et Metiers Hotel</t>
+          <t>Hotel 29 Lepic</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>US$3,971</t>
+          <t>US$3,442</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>8.2</t>
+          <t>8.1</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -699,132 +699,132 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2,030</t>
+          <t>1,989</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Hotel Puy De Dôme</t>
+          <t>Hotel Royal Mansart</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>US$3,771</t>
+          <t>US$2,290</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>8.1</t>
+          <t>7.3</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Very Good</t>
+          <t>Good</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>1,637</t>
+          <t>1,517</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Hotel Royal Phare</t>
+          <t>Hôtel La Conversation</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>US$3,701</t>
+          <t>US$4,005</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>8.3</t>
+          <t>9.0</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Very Good</t>
+          <t>Wonderful</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>1,735</t>
+          <t>91</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Hôtel San Régis</t>
+          <t>Hotel Flanelles Paris</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>US$24,224</t>
+          <t>US$3,884</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>8.9</t>
+          <t>8.4</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Excellent</t>
+          <t>Very Good</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>472</t>
+          <t>209</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Hotel Anya</t>
+          <t>Hôtel Lucien &amp; Marinette</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>US$1,918</t>
+          <t>US$3,283</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>7.4</t>
+          <t>8.2</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Good</t>
+          <t>Very Good</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>1,132</t>
+          <t>3,619</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>M Social Hotel Paris Opera</t>
+          <t>Baba Hotel</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>US$5,900</t>
+          <t>US$3,497</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>8.3</t>
+          <t>8.0</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -834,105 +834,105 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>1,445</t>
+          <t>261</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Hotel d'Orléans Paris Gare de l'Est</t>
+          <t>Auteuil Tour Eiffel</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>US$1,270</t>
+          <t>US$5,348</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>5.7</t>
+          <t>8.3</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Review score</t>
+          <t>Very Good</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>1,363</t>
+          <t>2,003</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Hotel Royal Mansart</t>
+          <t>La Belle Ville</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>US$2,290</t>
+          <t>US$4,212</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>7.3</t>
+          <t>8.7</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Good</t>
+          <t>Excellent</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>1,517</t>
+          <t>2,768</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>FM Hotel</t>
+          <t>Hotel Modern Est</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>US$1,570</t>
+          <t>US$2,831</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>3.6</t>
+          <t>7.9</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Review score</t>
+          <t>Good</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>853</t>
+          <t>2,374</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Studio - Butte aux cailles 13eme</t>
+          <t>Prince Albert Wagram</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>US$2,034</t>
+          <t>US$2,530</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>7.7</t>
+          <t>7.6</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -942,24 +942,24 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>1,375</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Hotel Eden Montmartre</t>
+          <t>Hotel Massena</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>US$2,438</t>
+          <t>US$4,400</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>7.9</t>
+          <t>7.8</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -969,51 +969,51 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>1,595</t>
+          <t>888</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Residence Les Boulevards</t>
+          <t>Hotel Royal Phare</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>US$3,140</t>
+          <t>US$3,701</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>7.8</t>
+          <t>8.3</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Good</t>
+          <t>Very Good</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>460</t>
+          <t>1,735</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Sure Hotel by Best Western Paris Gare du Nord</t>
+          <t>ATN Hôtel</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>US$2,213</t>
+          <t>US$3,237</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>7.0</t>
+          <t>7.9</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -1023,51 +1023,51 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>1,024</t>
+          <t>1,717</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Apart hotel Le Marais Centre de Paris</t>
+          <t>Hôtel Lumières Montmartre Paris</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>US$4,613</t>
+          <t>US$2,132</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>8.0</t>
+          <t>7.4</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Very Good</t>
+          <t>Good</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>163</t>
+          <t>1,799</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Hôtel Le M</t>
+          <t>Hotel L’Antoine</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>US$4,672</t>
+          <t>US$5,164</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>8.0</t>
+          <t>8.4</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -1077,24 +1077,24 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>1,485</t>
+          <t>1,332</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Hôtel De Castiglione</t>
+          <t>Residence Les Boulevards</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>US$4,559</t>
+          <t>US$3,140</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>7.5</t>
+          <t>7.8</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -1104,24 +1104,24 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>3,693</t>
+          <t>460</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Hôtel Des Fontaines</t>
+          <t>Apart hotel Louvre Centre de Paris (Pélican)</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>US$2,539</t>
+          <t>US$5,195</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>5.9</t>
+          <t>6.4</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -1131,7 +1131,7 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>473</t>
+          <t>45</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update hotel prices and scores in all_hotels.csv
</commit_message>
<xml_diff>
--- a/data/out/all_hotels.xlsx
+++ b/data/out/all_hotels.xlsx
@@ -463,71 +463,71 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Austin's Saint Lazare Hotel</t>
+          <t>Hôtel des Andelys</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>US$3,534</t>
+          <t>US$1,423</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>8.1</t>
+          <t>4.0</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Very Good</t>
+          <t>Review score</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2,540</t>
+          <t>929</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Austin's Arts Et Metiers Hotel</t>
+          <t>City Inn Paris</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>US$3,971</t>
+          <t>US$608</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>8.2</t>
+          <t>6.7</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Very Good</t>
+          <t>Review score</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2,030</t>
+          <t>2,498</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Apart hotel Le Marais Centre de Paris</t>
+          <t>Austin's Saint Lazare Hotel</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>US$4,613</t>
+          <t>US$3,534</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>8.0</t>
+          <t>8.1</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -537,105 +537,105 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>163</t>
+          <t>2,540</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Hotel Puy De Dôme</t>
+          <t>Auriane Porte De Versailles</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>US$3,771</t>
+          <t>US$1,948</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>8.1</t>
+          <t>5.6</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Very Good</t>
+          <t>Review score</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>1,637</t>
+          <t>1,636</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Hotel Anya</t>
+          <t>Zoku Paris</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>US$1,918</t>
+          <t>US$3,315</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>7.4</t>
+          <t>9.1</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Good</t>
+          <t>Wonderful</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>1,132</t>
+          <t>887</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>PARIS AUTHENTIC HOUSE, Entier 1920's villa métro Line 7</t>
+          <t>Hotel Royal Phare</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>US$10,710</t>
+          <t>US$3,701</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>9.4</t>
+          <t>8.3</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Wonderful</t>
+          <t>Very Good</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>1,735</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Zoku Paris</t>
+          <t>Hôtel La Conversation</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>US$3,315</t>
+          <t>US$4,005</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>9.1</t>
+          <t>9.0</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -645,186 +645,186 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>887</t>
+          <t>91</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Glasgow Monceau by Patrick Hayat</t>
+          <t>Hôtel de l'Aveyron</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>US$2,897</t>
+          <t>US$2,075</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>8.0</t>
+          <t>6.1</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Very Good</t>
+          <t>Review score</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>674</t>
+          <t>2,077</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Hotel 29 Lepic</t>
+          <t>Hotel Anya</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>US$3,442</t>
+          <t>US$1,918</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>8.1</t>
+          <t>7.4</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Very Good</t>
+          <t>Good</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>1,989</t>
+          <t>1,132</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Hotel Royal Mansart</t>
+          <t>Glasgow Monceau by Patrick Hayat</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>US$2,290</t>
+          <t>US$2,897</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>7.3</t>
+          <t>8.0</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Good</t>
+          <t>Very Good</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>1,517</t>
+          <t>674</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Hôtel La Conversation</t>
+          <t>Printania Porte de Versailles</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>US$4,005</t>
+          <t>US$1,948</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>9.0</t>
+          <t>5.7</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Wonderful</t>
+          <t>Review score</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>91</t>
+          <t>1,284</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Hotel Flanelles Paris</t>
+          <t>PORTE MAILLOT CHAMPS ELYSÉES PARIS</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>US$3,884</t>
+          <t>US$3,469</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>8.4</t>
+          <t>4.7</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Very Good</t>
+          <t>Review score</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>209</t>
+          <t>3</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Hôtel Lucien &amp; Marinette</t>
+          <t>STYLE HOTEL</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>US$3,283</t>
+          <t>US$1,939</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>8.2</t>
+          <t>6.0</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Very Good</t>
+          <t>Review score</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>3,619</t>
+          <t>744</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Baba Hotel</t>
+          <t>Austin's Arts Et Metiers Hotel</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>US$3,497</t>
+          <t>US$3,971</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>8.0</t>
+          <t>8.2</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -834,294 +834,282 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>261</t>
+          <t>2,030</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Auteuil Tour Eiffel</t>
+          <t>Hôtel De Castiglione</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>US$5,348</t>
+          <t>US$4,559</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>8.3</t>
+          <t>7.5</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Very Good</t>
+          <t>Good</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>2,003</t>
+          <t>3,693</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>La Belle Ville</t>
+          <t>FM Hotel</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>US$4,212</t>
+          <t>US$1,570</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>8.7</t>
+          <t>3.6</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Excellent</t>
+          <t>Review score</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>2,768</t>
+          <t>853</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Hotel Modern Est</t>
+          <t>Charmant studio grand balcon parking</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>US$2,831</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>7.9</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>Good</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>2,374</t>
-        </is>
-      </c>
+          <t>US$2,179</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr"/>
+      <c r="D18" t="inlineStr"/>
+      <c r="E18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Prince Albert Wagram</t>
+          <t>Aparthotel Adagio Paris Buttes Chaumont</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>US$2,530</t>
+          <t>US$4,354</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>7.6</t>
+          <t>8.3</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Good</t>
+          <t>Very Good</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>1,375</t>
+          <t>562</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Hotel Massena</t>
+          <t>Apart hotel Le Marais Centre de Paris</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>US$4,400</t>
+          <t>US$4,613</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>7.8</t>
+          <t>8.0</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Good</t>
+          <t>Very Good</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>888</t>
+          <t>163</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Hotel Royal Phare</t>
+          <t>Studio - Butte aux cailles 13eme</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>US$3,701</t>
+          <t>US$2,034</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>8.3</t>
+          <t>7.7</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Very Good</t>
+          <t>Good</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>1,735</t>
+          <t>9</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>ATN Hôtel</t>
+          <t>HOTEL SAVOY</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>US$3,237</t>
+          <t>US$1,575</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>7.9</t>
+          <t>6.1</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Good</t>
+          <t>Review score</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>1,717</t>
+          <t>779</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Hôtel Lumières Montmartre Paris</t>
+          <t>Hôtel Des Fontaines</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>US$2,132</t>
+          <t>US$2,539</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>7.4</t>
+          <t>5.9</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Good</t>
+          <t>Review score</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>1,799</t>
+          <t>473</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Hotel L’Antoine</t>
+          <t>Hotel Eden Montmartre</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>US$5,164</t>
+          <t>US$2,438</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>8.4</t>
+          <t>7.9</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Very Good</t>
+          <t>Good</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>1,332</t>
+          <t>1,595</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Residence Les Boulevards</t>
+          <t>Domitys L'Ellipse</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>US$3,140</t>
+          <t>US$2,977</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>7.8</t>
+          <t>9.2</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Good</t>
+          <t>Wonderful</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>460</t>
+          <t>6</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Apart hotel Louvre Centre de Paris (Pélican)</t>
+          <t>Hotel de France 18</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>US$5,195</t>
+          <t>US$1,279</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>6.4</t>
+          <t>6.0</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -1131,7 +1119,7 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>45</t>
+          <t>1,891</t>
         </is>
       </c>
     </row>

</xml_diff>